<commit_message>
Added comments + Made StudHelper class as Singleton
</commit_message>
<xml_diff>
--- a/Tested Files/testSH.xlsx
+++ b/Tested Files/testSH.xlsx
@@ -426,16 +426,25 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
+        <v>2</v>
+      </c>
+      <c r="B4">
         <v>2</v>
       </c>
     </row>
@@ -444,11 +453,17 @@
         <f aca="false">RANDBETWEEN(1,4)</f>
         <v>1</v>
       </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,4)</f>
         <v>3</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>